<commit_message>
Adding information about WHO.
</commit_message>
<xml_diff>
--- a/data_output/PYLL/PYLL_EU/EU_ASYR_(0-4)-(85-89)_['Female', 'Male', 'Total'].xlsx
+++ b/data_output/PYLL/PYLL_EU/EU_ASYR_(0-4)-(85-89)_['Female', 'Male', 'Total'].xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="37">
   <si>
     <t>Location</t>
   </si>
@@ -28,12 +28,6 @@
     <t>ASYR_FLUC</t>
   </si>
   <si>
-    <t>Albania</t>
-  </si>
-  <si>
-    <t>Armenia</t>
-  </si>
-  <si>
     <t>Austria</t>
   </si>
   <si>
@@ -62,12 +56,6 @@
   </si>
   <si>
     <t>France</t>
-  </si>
-  <si>
-    <t>Georgia</t>
-  </si>
-  <si>
-    <t>Germany</t>
   </si>
   <si>
     <t>Greece</t>
@@ -494,7 +482,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:D91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -519,13 +507,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C2">
-        <v>1280.079</v>
+        <v>700.063</v>
       </c>
       <c r="D2">
-        <v>334.028</v>
+        <v>591.9300000000001</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -533,13 +521,13 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C3">
-        <v>3397.134</v>
+        <v>1289.23</v>
       </c>
       <c r="D3">
-        <v>448.809</v>
+        <v>663.831</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -547,13 +535,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C4">
-        <v>2313.455</v>
+        <v>949.274</v>
       </c>
       <c r="D4">
-        <v>337.8939999999999</v>
+        <v>459.687</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -561,13 +549,13 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C5">
-        <v>2679.467</v>
+        <v>1018.067</v>
       </c>
       <c r="D5">
-        <v>419.1659999999999</v>
+        <v>473.256</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -575,13 +563,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C6">
-        <v>10902.035</v>
+        <v>1749.278</v>
       </c>
       <c r="D6">
-        <v>742.0229999999999</v>
+        <v>668.5410000000001</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -589,13 +577,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C7">
-        <v>6887.798000000001</v>
+        <v>1392.44</v>
       </c>
       <c r="D7">
-        <v>519.245</v>
+        <v>450.33</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -603,13 +591,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C8">
-        <v>626.6709999999998</v>
+        <v>2429.858</v>
       </c>
       <c r="D8">
-        <v>216.956</v>
+        <v>799.681</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -617,13 +605,13 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C9">
-        <v>1237.816</v>
+        <v>4090.682</v>
       </c>
       <c r="D9">
-        <v>346.564</v>
+        <v>1022.675</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -631,13 +619,13 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C10">
-        <v>881.123</v>
+        <v>3251.429</v>
       </c>
       <c r="D10">
-        <v>251.162</v>
+        <v>678.16</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -645,13 +633,13 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C11">
-        <v>861.854</v>
+        <v>1295.691</v>
       </c>
       <c r="D11">
-        <v>244.811</v>
+        <v>974.8870000000001</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -659,13 +647,13 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C12">
-        <v>1407.019</v>
+        <v>2017.011</v>
       </c>
       <c r="D12">
-        <v>347.931</v>
+        <v>1021.732</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -673,13 +661,13 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C13">
-        <v>1119.255</v>
+        <v>1604.407</v>
       </c>
       <c r="D13">
-        <v>277.939</v>
+        <v>797.638</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -687,13 +675,13 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C14">
-        <v>2028.106</v>
+        <v>503.248</v>
       </c>
       <c r="D14">
-        <v>341.085</v>
+        <v>1058.958</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -701,13 +689,13 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C15">
-        <v>3653.955</v>
+        <v>544.582</v>
       </c>
       <c r="D15">
-        <v>510.354</v>
+        <v>1219.26</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -715,13 +703,13 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C16">
-        <v>2826.968</v>
+        <v>430.07</v>
       </c>
       <c r="D16">
-        <v>403.9519999999999</v>
+        <v>797.274</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -729,13 +717,13 @@
         <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C17">
-        <v>755.905</v>
+        <v>1262.004</v>
       </c>
       <c r="D17">
-        <v>346.106</v>
+        <v>630.8100000000001</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -743,13 +731,13 @@
         <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C18">
-        <v>1439.726</v>
+        <v>2223.926</v>
       </c>
       <c r="D18">
-        <v>384.641</v>
+        <v>757.554</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -757,13 +745,13 @@
         <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C19">
-        <v>1064.612</v>
+        <v>1709.024</v>
       </c>
       <c r="D19">
-        <v>320.002</v>
+        <v>484.859</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -771,13 +759,13 @@
         <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C20">
-        <v>546.2150000000001</v>
+        <v>268.875</v>
       </c>
       <c r="D20">
-        <v>306.535</v>
+        <v>599.635</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -785,13 +773,13 @@
         <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C21">
-        <v>1156.146</v>
+        <v>292.626</v>
       </c>
       <c r="D21">
-        <v>595.4850000000001</v>
+        <v>634.605</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -799,13 +787,13 @@
         <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C22">
-        <v>806.026</v>
+        <v>236.146</v>
       </c>
       <c r="D22">
-        <v>339.676</v>
+        <v>482.905</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -813,13 +801,13 @@
         <v>11</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C23">
-        <v>1206.8</v>
+        <v>781.346</v>
       </c>
       <c r="D23">
-        <v>311.302</v>
+        <v>1349.463</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -827,13 +815,13 @@
         <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C24">
-        <v>2332.294</v>
+        <v>1178.006</v>
       </c>
       <c r="D24">
-        <v>430.6180000000001</v>
+        <v>1964.719</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -841,13 +829,13 @@
         <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C25">
-        <v>1725.248</v>
+        <v>865.9880000000001</v>
       </c>
       <c r="D25">
-        <v>351.772</v>
+        <v>1359.787</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -855,13 +843,13 @@
         <v>12</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C26">
-        <v>263.7859999999999</v>
+        <v>229.715</v>
       </c>
       <c r="D26">
-        <v>95.77200000000001</v>
+        <v>527.529</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -869,13 +857,13 @@
         <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C27">
-        <v>456.2119999999999</v>
+        <v>590.3680000000001</v>
       </c>
       <c r="D27">
-        <v>169.323</v>
+        <v>764.304</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -883,13 +871,13 @@
         <v>12</v>
       </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C28">
-        <v>344.816</v>
+        <v>354.5</v>
       </c>
       <c r="D28">
-        <v>146.967</v>
+        <v>510.806</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -897,13 +885,13 @@
         <v>13</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C29">
-        <v>724.1210000000001</v>
+        <v>446.025</v>
       </c>
       <c r="D29">
-        <v>403.42</v>
+        <v>207.977</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -911,13 +899,13 @@
         <v>13</v>
       </c>
       <c r="B30" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C30">
-        <v>976.073</v>
+        <v>1047.717</v>
       </c>
       <c r="D30">
-        <v>492.727</v>
+        <v>291.137</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -925,13 +913,13 @@
         <v>13</v>
       </c>
       <c r="B31" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C31">
-        <v>772.2090000000001</v>
+        <v>737.08</v>
       </c>
       <c r="D31">
-        <v>404.0860000000001</v>
+        <v>211.755</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -939,13 +927,13 @@
         <v>14</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C32">
-        <v>322.342</v>
+        <v>533.4400000000001</v>
       </c>
       <c r="D32">
-        <v>163.008</v>
+        <v>483.097</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -953,13 +941,13 @@
         <v>14</v>
       </c>
       <c r="B33" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C33">
-        <v>591.615</v>
+        <v>746.981</v>
       </c>
       <c r="D33">
-        <v>214.414</v>
+        <v>590.7430000000001</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -967,13 +955,13 @@
         <v>14</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C34">
-        <v>444.3320000000001</v>
+        <v>615.7280000000001</v>
       </c>
       <c r="D34">
-        <v>172.756</v>
+        <v>395.739</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -981,13 +969,13 @@
         <v>15</v>
       </c>
       <c r="B35" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C35">
-        <v>479.79</v>
+        <v>1468.783</v>
       </c>
       <c r="D35">
-        <v>127.463</v>
+        <v>717.03</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -995,13 +983,13 @@
         <v>15</v>
       </c>
       <c r="B36" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C36">
-        <v>916.442</v>
+        <v>2069.63</v>
       </c>
       <c r="D36">
-        <v>218.078</v>
+        <v>949.075</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1009,13 +997,13 @@
         <v>15</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C37">
-        <v>686.8950000000001</v>
+        <v>1745.198</v>
       </c>
       <c r="D37">
-        <v>171.353</v>
+        <v>682.03</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1023,13 +1011,13 @@
         <v>16</v>
       </c>
       <c r="B38" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C38">
-        <v>62.218</v>
+        <v>766.3440000000001</v>
       </c>
       <c r="D38">
-        <v>89.501</v>
+        <v>1462.581</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1037,13 +1025,13 @@
         <v>16</v>
       </c>
       <c r="B39" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C39">
-        <v>181.085</v>
+        <v>992.335</v>
       </c>
       <c r="D39">
-        <v>142.362</v>
+        <v>2233.389</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1051,13 +1039,13 @@
         <v>16</v>
       </c>
       <c r="B40" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C40">
-        <v>96.95</v>
+        <v>673.2329999999999</v>
       </c>
       <c r="D40">
-        <v>104.848</v>
+        <v>1459.186</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1065,41 +1053,41 @@
         <v>17</v>
       </c>
       <c r="B41" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C41">
-        <v>772.2809999999999</v>
+        <v>871.088</v>
       </c>
       <c r="D41">
-        <v>2416.067</v>
+        <v>207.263</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B42" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C42">
-        <v>408.4920000000001</v>
+        <v>1841.612</v>
       </c>
       <c r="D42">
-        <v>178.966</v>
+        <v>275.824</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B43" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C43">
-        <v>538.917</v>
+        <v>1520.923</v>
       </c>
       <c r="D43">
-        <v>153.091</v>
+        <v>221.525</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1107,41 +1095,41 @@
         <v>18</v>
       </c>
       <c r="B44" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C44">
-        <v>460.89</v>
+        <v>751.279</v>
       </c>
       <c r="D44">
-        <v>160.035</v>
+        <v>1060.349</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B45" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C45">
-        <v>1211.734</v>
+        <v>1194.318</v>
       </c>
       <c r="D45">
-        <v>239.06</v>
+        <v>1774.912</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B46" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C46">
-        <v>1859.083</v>
+        <v>945.0179999999999</v>
       </c>
       <c r="D46">
-        <v>372.379</v>
+        <v>1119.654</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1149,41 +1137,41 @@
         <v>19</v>
       </c>
       <c r="B47" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C47">
-        <v>1505.23</v>
+        <v>2066.8</v>
       </c>
       <c r="D47">
-        <v>268.73</v>
+        <v>1246.048</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B48" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C48">
-        <v>616.5640000000001</v>
+        <v>4863.499</v>
       </c>
       <c r="D48">
-        <v>380.277</v>
+        <v>1980.009</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B49" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C49">
-        <v>1200.438</v>
+        <v>3430.524</v>
       </c>
       <c r="D49">
-        <v>587.433</v>
+        <v>1262.209</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1191,41 +1179,41 @@
         <v>20</v>
       </c>
       <c r="B50" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C50">
-        <v>762.275</v>
+        <v>707.668</v>
       </c>
       <c r="D50">
-        <v>456.929</v>
+        <v>1537.727</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B51" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C51">
-        <v>610.885</v>
+        <v>1302.231</v>
       </c>
       <c r="D51">
-        <v>156.225</v>
+        <v>1888.576</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B52" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C52">
-        <v>1436.499</v>
+        <v>891.451</v>
       </c>
       <c r="D52">
-        <v>203.037</v>
+        <v>1401.15</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1233,41 +1221,41 @@
         <v>21</v>
       </c>
       <c r="B53" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C53">
-        <v>1183.668</v>
+        <v>984.6609999999999</v>
       </c>
       <c r="D53">
-        <v>189.976</v>
+        <v>1815.822</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B54" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C54">
-        <v>242.098</v>
+        <v>1257.279</v>
       </c>
       <c r="D54">
-        <v>137.731</v>
+        <v>2011.675</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B55" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C55">
-        <v>645.9359999999999</v>
+        <v>1077.857</v>
       </c>
       <c r="D55">
-        <v>363.638</v>
+        <v>1540.395</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1275,41 +1263,41 @@
         <v>22</v>
       </c>
       <c r="B56" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C56">
-        <v>383.966</v>
+        <v>2021.572</v>
       </c>
       <c r="D56">
-        <v>250.057</v>
+        <v>2453.438</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B57" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C57">
-        <v>1046.42</v>
+        <v>2896.193</v>
       </c>
       <c r="D57">
-        <v>470.446</v>
+        <v>2031.353</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B58" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C58">
-        <v>2290.376</v>
+        <v>2309.043</v>
       </c>
       <c r="D58">
-        <v>1008.833</v>
+        <v>1633.625</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1317,41 +1305,41 @@
         <v>23</v>
       </c>
       <c r="B59" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C59">
-        <v>1608.274</v>
+        <v>624.254</v>
       </c>
       <c r="D59">
-        <v>732.3230000000001</v>
+        <v>365.482</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B60" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C60">
-        <v>810.9390000000001</v>
+        <v>1252.94</v>
       </c>
       <c r="D60">
-        <v>464.2860000000001</v>
+        <v>459.886</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B61" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C61">
-        <v>1389.716</v>
+        <v>931.11</v>
       </c>
       <c r="D61">
-        <v>814.813</v>
+        <v>337.633</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1359,41 +1347,41 @@
         <v>24</v>
       </c>
       <c r="B62" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C62">
-        <v>1016.74</v>
+        <v>101.996</v>
       </c>
       <c r="D62">
-        <v>583.1560000000001</v>
+        <v>395.017</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B63" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C63">
-        <v>861.3300000000003</v>
+        <v>206.297</v>
       </c>
       <c r="D63">
-        <v>586.0069999999999</v>
+        <v>592.5840000000001</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B64" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C64">
-        <v>1755.687</v>
+        <v>121.097</v>
       </c>
       <c r="D64">
-        <v>723.266</v>
+        <v>372.628</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1401,41 +1389,41 @@
         <v>25</v>
       </c>
       <c r="B65" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C65">
-        <v>1278.732</v>
+        <v>1494.848</v>
       </c>
       <c r="D65">
-        <v>560.9440000000001</v>
+        <v>385.588</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B66" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C66">
-        <v>1232.941</v>
+        <v>3218.766</v>
       </c>
       <c r="D66">
-        <v>442.477</v>
+        <v>525.948</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B67" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C67">
-        <v>2404.332</v>
+        <v>2328.762</v>
       </c>
       <c r="D67">
-        <v>936.2669999999999</v>
+        <v>372.609</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1443,41 +1431,41 @@
         <v>26</v>
       </c>
       <c r="B68" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C68">
-        <v>1740.853</v>
+        <v>796.614</v>
       </c>
       <c r="D68">
-        <v>490.595</v>
+        <v>499.839</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B69" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C69">
-        <v>702.2090000000001</v>
+        <v>1232.932</v>
       </c>
       <c r="D69">
-        <v>200.2130000000001</v>
+        <v>769.996</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B70" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C70">
-        <v>1341.706</v>
+        <v>1004.958</v>
       </c>
       <c r="D70">
-        <v>250.376</v>
+        <v>518.894</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -1485,41 +1473,41 @@
         <v>27</v>
       </c>
       <c r="B71" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C71">
-        <v>991.724</v>
+        <v>1986.148</v>
       </c>
       <c r="D71">
-        <v>221.407</v>
+        <v>592.946</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B72" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C72">
-        <v>183.495</v>
+        <v>3363.22</v>
       </c>
       <c r="D72">
-        <v>154.174</v>
+        <v>795.504</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B73" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C73">
-        <v>278.952</v>
+        <v>2632.306</v>
       </c>
       <c r="D73">
-        <v>142.06</v>
+        <v>558.639</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -1527,41 +1515,41 @@
         <v>28</v>
       </c>
       <c r="B74" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C74">
-        <v>222.38</v>
+        <v>1382.796</v>
       </c>
       <c r="D74">
-        <v>142.155</v>
+        <v>777.1660000000001</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B75" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C75">
-        <v>1558.014</v>
+        <v>3073.032</v>
       </c>
       <c r="D75">
-        <v>350.712</v>
+        <v>1099.285</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B76" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C76">
-        <v>3303.545000000001</v>
+        <v>2180.531</v>
       </c>
       <c r="D76">
-        <v>554.38</v>
+        <v>785.601</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -1569,41 +1557,41 @@
         <v>29</v>
       </c>
       <c r="B77" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C77">
-        <v>2385.461</v>
+        <v>1387.476</v>
       </c>
       <c r="D77">
-        <v>442.179</v>
+        <v>851.309</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B78" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C78">
-        <v>677.5080000000002</v>
+        <v>2075.769</v>
       </c>
       <c r="D78">
-        <v>204.513</v>
+        <v>1209.447</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B79" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C79">
-        <v>1170.435</v>
+        <v>1689.908</v>
       </c>
       <c r="D79">
-        <v>321.333</v>
+        <v>793.482</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -1611,41 +1599,41 @@
         <v>30</v>
       </c>
       <c r="B80" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C80">
-        <v>918.551</v>
+        <v>1195.765</v>
       </c>
       <c r="D80">
-        <v>205.981</v>
+        <v>871.761</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B81" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C81">
-        <v>1520.329</v>
+        <v>1969.012</v>
       </c>
       <c r="D81">
-        <v>316.263</v>
+        <v>1411.741</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B82" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C82">
-        <v>3214.981</v>
+        <v>1559.112</v>
       </c>
       <c r="D82">
-        <v>519.442</v>
+        <v>839.878</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -1653,41 +1641,41 @@
         <v>31</v>
       </c>
       <c r="B83" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C83">
-        <v>2353.129</v>
+        <v>1122.042</v>
       </c>
       <c r="D83">
-        <v>402.178</v>
+        <v>266.348</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B84" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C84">
-        <v>839.1959999999999</v>
+        <v>1869.329</v>
       </c>
       <c r="D84">
-        <v>297.189</v>
+        <v>356.136</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B85" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C85">
-        <v>2323.639</v>
+        <v>1503.876</v>
       </c>
       <c r="D85">
-        <v>723.3580000000001</v>
+        <v>243.176</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -1695,41 +1683,41 @@
         <v>32</v>
       </c>
       <c r="B86" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C86">
-        <v>1498.929</v>
+        <v>491.9299999999999</v>
       </c>
       <c r="D86">
-        <v>460.079</v>
+        <v>398.334</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B87" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C87">
-        <v>1170.017</v>
+        <v>1210.012</v>
       </c>
       <c r="D87">
-        <v>345.856</v>
+        <v>580.277</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B88" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C88">
-        <v>2094.6</v>
+        <v>830.6270000000001</v>
       </c>
       <c r="D88">
-        <v>339.314</v>
+        <v>399.182</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -1737,181 +1725,41 @@
         <v>33</v>
       </c>
       <c r="B89" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C89">
-        <v>1555.849</v>
+        <v>348.648</v>
       </c>
       <c r="D89">
-        <v>239.553</v>
+        <v>490.94</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B90" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C90">
-        <v>997.1990000000001</v>
+        <v>989.759</v>
       </c>
       <c r="D90">
-        <v>298.806</v>
+        <v>702.8869999999999</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B91" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C91">
-        <v>1837.148</v>
+        <v>647.862</v>
       </c>
       <c r="D91">
-        <v>460.418</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4">
-      <c r="A92" t="s">
-        <v>34</v>
-      </c>
-      <c r="B92" t="s">
-        <v>40</v>
-      </c>
-      <c r="C92">
-        <v>1364.685</v>
-      </c>
-      <c r="D92">
-        <v>285.693</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4">
-      <c r="A93" t="s">
-        <v>35</v>
-      </c>
-      <c r="B93" t="s">
-        <v>38</v>
-      </c>
-      <c r="C93">
-        <v>1015.775</v>
-      </c>
-      <c r="D93">
-        <v>176.354</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4">
-      <c r="A94" t="s">
-        <v>35</v>
-      </c>
-      <c r="B94" t="s">
-        <v>39</v>
-      </c>
-      <c r="C94">
-        <v>1698.117</v>
-      </c>
-      <c r="D94">
-        <v>247.489</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4">
-      <c r="A95" t="s">
-        <v>35</v>
-      </c>
-      <c r="B95" t="s">
-        <v>40</v>
-      </c>
-      <c r="C95">
-        <v>1355.724</v>
-      </c>
-      <c r="D95">
-        <v>204.065</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4">
-      <c r="A96" t="s">
-        <v>36</v>
-      </c>
-      <c r="B96" t="s">
-        <v>38</v>
-      </c>
-      <c r="C96">
-        <v>437.297</v>
-      </c>
-      <c r="D96">
-        <v>100.668</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4">
-      <c r="A97" t="s">
-        <v>36</v>
-      </c>
-      <c r="B97" t="s">
-        <v>39</v>
-      </c>
-      <c r="C97">
-        <v>815.687</v>
-      </c>
-      <c r="D97">
-        <v>199.025</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4">
-      <c r="A98" t="s">
-        <v>36</v>
-      </c>
-      <c r="B98" t="s">
-        <v>40</v>
-      </c>
-      <c r="C98">
-        <v>579.422</v>
-      </c>
-      <c r="D98">
-        <v>120.346</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4">
-      <c r="A99" t="s">
-        <v>37</v>
-      </c>
-      <c r="B99" t="s">
-        <v>38</v>
-      </c>
-      <c r="C99">
-        <v>393.086</v>
-      </c>
-      <c r="D99">
-        <v>100.596</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4">
-      <c r="A100" t="s">
-        <v>37</v>
-      </c>
-      <c r="B100" t="s">
-        <v>39</v>
-      </c>
-      <c r="C100">
-        <v>855.283</v>
-      </c>
-      <c r="D100">
-        <v>255.798</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4">
-      <c r="A101" t="s">
-        <v>37</v>
-      </c>
-      <c r="B101" t="s">
-        <v>40</v>
-      </c>
-      <c r="C101">
-        <v>579.9160000000001</v>
-      </c>
-      <c r="D101">
-        <v>171.308</v>
+        <v>473.248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>